<commit_message>
add the execl file for Renesas ISL8273 and UCD9090 voltage hex value
</commit_message>
<xml_diff>
--- a/truck/doc/Renesas_ISL8273_vset.xlsx
+++ b/truck/doc/Renesas_ISL8273_vset.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Renesas ISL8273 Vout setting</t>
   </si>
@@ -98,13 +98,21 @@
   </si>
   <si>
     <t>#i2cset -f -y 1 0x1A 0x21 0x1E66 w</t>
+  </si>
+  <si>
+    <t>isl8273</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ucd9090</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -149,6 +157,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -164,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -296,13 +313,289 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -333,18 +626,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -371,6 +655,96 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -652,10 +1026,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U20"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U32" sqref="U32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -665,21 +1039,24 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.25" customWidth="1"/>
-    <col min="15" max="15" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="15.25" customWidth="1"/>
+    <col min="16" max="16" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.25" customWidth="1"/>
+    <col min="19" max="19" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.875" customWidth="1"/>
+    <col min="22" max="22" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.25" customWidth="1"/>
+    <col min="25" max="25" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -690,7 +1067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="str">
         <f>DEC2HEX(B3)</f>
         <v>1E66</v>
@@ -703,7 +1080,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="str">
         <f t="shared" ref="A4:A14" si="0">DEC2HEX(B4)</f>
         <v>1EB8</v>
@@ -716,7 +1093,7 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="str">
         <f t="shared" si="0"/>
         <v>1F0A</v>
@@ -729,7 +1106,7 @@
         <v>0.97</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="str">
         <f t="shared" si="0"/>
         <v>1F5C</v>
@@ -742,7 +1119,7 @@
         <v>0.98</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="str">
         <f t="shared" si="0"/>
         <v>1FAE</v>
@@ -754,31 +1131,53 @@
       <c r="C7" s="8">
         <v>0.99</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9">
+      <c r="I7" s="40"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="42">
         <v>1.1499999999999999</v>
       </c>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9">
+      <c r="M7" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="O7" s="9"/>
-      <c r="P7" s="9">
+      <c r="P7" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q7" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="R7" s="43">
         <v>0.85</v>
       </c>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9">
+      <c r="S7" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="T7" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="U7" s="43">
         <v>0.9</v>
       </c>
-      <c r="S7" s="9"/>
-      <c r="T7" s="9">
+      <c r="V7" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="W7" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="X7" s="43">
         <v>1.1000000000000001</v>
       </c>
-      <c r="U7" s="9"/>
+      <c r="Y7" s="32" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="8" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="str">
         <f t="shared" si="0"/>
         <v>2000</v>
@@ -790,43 +1189,47 @@
       <c r="C8" s="8">
         <v>1</v>
       </c>
-      <c r="I8" s="9"/>
+      <c r="I8" s="24"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="L8" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="M8" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="N8" s="38"/>
+      <c r="O8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="O8" s="9" t="s">
+      <c r="P8" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="P8" s="9" t="s">
+      <c r="Q8" s="38"/>
+      <c r="R8" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="9" t="s">
+      <c r="S8" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="T8" s="38"/>
+      <c r="U8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="S8" s="9" t="s">
+      <c r="V8" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="T8" s="9" t="s">
+      <c r="W8" s="38"/>
+      <c r="X8" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="U8" s="9" t="s">
+      <c r="Y8" s="35" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="str">
         <f t="shared" si="0"/>
         <v>2051</v>
@@ -838,59 +1241,75 @@
       <c r="C9" s="8">
         <v>1.01</v>
       </c>
-      <c r="I9" s="10" t="str">
+      <c r="I9" s="44" t="str">
         <f>DEC2HEX(J9)</f>
         <v>1E66</v>
       </c>
-      <c r="J9" s="11">
+      <c r="J9" s="10">
         <f>K9/2^(-13)</f>
         <v>7782.4</v>
       </c>
-      <c r="K9" s="11">
+      <c r="K9" s="10">
         <v>0.95</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="21">
         <f>K9*1.15</f>
         <v>1.0924999999999998</v>
       </c>
-      <c r="M9" s="12" t="str">
+      <c r="M9" s="36" t="str">
         <f>DEC2HEX(L9/2^(-13))</f>
         <v>22F5</v>
       </c>
-      <c r="N9" s="12">
+      <c r="N9" s="37" t="str">
+        <f>DEC2HEX(L9/2^(-14))</f>
+        <v>45EB</v>
+      </c>
+      <c r="O9" s="31">
         <f>K9*1.1</f>
         <v>1.0449999999999999</v>
       </c>
-      <c r="O9" s="12" t="str">
-        <f>DEC2HEX(N9/2^(-13))</f>
+      <c r="P9" s="36" t="str">
+        <f>DEC2HEX(O9/2^(-13))</f>
         <v>2170</v>
       </c>
-      <c r="P9" s="12">
+      <c r="Q9" s="37" t="str">
+        <f>DEC2HEX(O9/2^(-14))</f>
+        <v>42E1</v>
+      </c>
+      <c r="R9" s="31">
         <f>K9*0.85</f>
         <v>0.8075</v>
       </c>
-      <c r="Q9" s="12" t="str">
-        <f>DEC2HEX(P9/2^(-13))</f>
+      <c r="S9" s="36" t="str">
+        <f>DEC2HEX(R9/2^(-13))</f>
         <v>19D7</v>
       </c>
-      <c r="R9" s="12">
+      <c r="T9" s="37" t="str">
+        <f>DEC2HEX(R9/2^(-14))</f>
+        <v>33AE</v>
+      </c>
+      <c r="U9" s="31">
         <f>K9*0.9</f>
         <v>0.85499999999999998</v>
       </c>
-      <c r="S9" s="12" t="str">
-        <f>DEC2HEX(R9/2^(-13))</f>
+      <c r="V9" s="36" t="str">
+        <f>DEC2HEX(U9/2^(-13))</f>
         <v>1B5C</v>
       </c>
-      <c r="T9" s="12">
+      <c r="W9" s="37" t="str">
+        <f>DEC2HEX(U9/2^(-14))</f>
+        <v>36B8</v>
+      </c>
+      <c r="X9" s="31">
         <f>K9*1.1</f>
         <v>1.0449999999999999</v>
       </c>
-      <c r="U9" s="12" t="str">
-        <f>DEC2HEX(T9/2^(-13))</f>
+      <c r="Y9" s="39" t="str">
+        <f>DEC2HEX(X9/2^(-13))</f>
         <v>2170</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="str">
         <f t="shared" si="0"/>
         <v>20A3</v>
@@ -902,59 +1321,75 @@
       <c r="C10" s="8">
         <v>1.02</v>
       </c>
-      <c r="I10" s="13" t="str">
+      <c r="I10" s="45" t="str">
         <f t="shared" ref="I10:I20" si="2">DEC2HEX(J10)</f>
         <v>1EB8</v>
       </c>
-      <c r="J10" s="14">
+      <c r="J10" s="11">
         <f t="shared" ref="J10:J20" si="3">K10/2^(-13)</f>
         <v>7864.32</v>
       </c>
-      <c r="K10" s="14">
+      <c r="K10" s="11">
         <v>0.96</v>
       </c>
-      <c r="L10" s="9">
+      <c r="L10" s="20">
         <f t="shared" ref="L10:L20" si="4">K10*1.15</f>
         <v>1.1039999999999999</v>
       </c>
-      <c r="M10" s="9" t="str">
+      <c r="M10" s="24" t="str">
         <f t="shared" ref="M10:M20" si="5">DEC2HEX(L10/2^(-13))</f>
         <v>2353</v>
       </c>
-      <c r="N10" s="9">
-        <f t="shared" ref="N10:N20" si="6">K10*1.1</f>
+      <c r="N10" s="27" t="str">
+        <f t="shared" ref="N10:N20" si="6">DEC2HEX(L10/2^(-14))</f>
+        <v>46A7</v>
+      </c>
+      <c r="O10" s="30">
+        <f t="shared" ref="O10:O20" si="7">K10*1.1</f>
         <v>1.056</v>
       </c>
-      <c r="O10" s="9" t="str">
-        <f t="shared" ref="O10:O20" si="7">DEC2HEX(N10/2^(-13))</f>
+      <c r="P10" s="24" t="str">
+        <f t="shared" ref="P10:P20" si="8">DEC2HEX(O10/2^(-13))</f>
         <v>21CA</v>
       </c>
-      <c r="P10" s="9">
-        <f t="shared" ref="P10:P20" si="8">K10*0.85</f>
+      <c r="Q10" s="27" t="str">
+        <f t="shared" ref="Q10:Q20" si="9">DEC2HEX(O10/2^(-14))</f>
+        <v>4395</v>
+      </c>
+      <c r="R10" s="30">
+        <f t="shared" ref="R10:R20" si="10">K10*0.85</f>
         <v>0.81599999999999995</v>
       </c>
-      <c r="Q10" s="9" t="str">
-        <f t="shared" ref="Q10:Q20" si="9">DEC2HEX(P10/2^(-13))</f>
+      <c r="S10" s="24" t="str">
+        <f t="shared" ref="S10:S20" si="11">DEC2HEX(R10/2^(-13))</f>
         <v>1A1C</v>
       </c>
-      <c r="R10" s="9">
-        <f t="shared" ref="R10:R20" si="10">K10*0.9</f>
+      <c r="T10" s="27" t="str">
+        <f t="shared" ref="T10:T20" si="12">DEC2HEX(R10/2^(-14))</f>
+        <v>3439</v>
+      </c>
+      <c r="U10" s="30">
+        <f t="shared" ref="U10:U20" si="13">K10*0.9</f>
         <v>0.86399999999999999</v>
       </c>
-      <c r="S10" s="9" t="str">
-        <f t="shared" ref="S10:S20" si="11">DEC2HEX(R10/2^(-13))</f>
+      <c r="V10" s="24" t="str">
+        <f t="shared" ref="V10:V20" si="14">DEC2HEX(U10/2^(-13))</f>
         <v>1BA5</v>
       </c>
-      <c r="T10" s="9">
-        <f t="shared" ref="T10:T20" si="12">K10*1.1</f>
+      <c r="W10" s="27" t="str">
+        <f t="shared" ref="W10:W20" si="15">DEC2HEX(U10/2^(-14))</f>
+        <v>374B</v>
+      </c>
+      <c r="X10" s="30">
+        <f t="shared" ref="X10:X20" si="16">K10*1.1</f>
         <v>1.056</v>
       </c>
-      <c r="U10" s="9" t="str">
-        <f t="shared" ref="U10:U20" si="13">DEC2HEX(T10/2^(-13))</f>
+      <c r="Y10" s="33" t="str">
+        <f t="shared" ref="Y10:Y20" si="17">DEC2HEX(X10/2^(-13))</f>
         <v>21CA</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="str">
         <f t="shared" si="0"/>
         <v>20F5</v>
@@ -966,59 +1401,75 @@
       <c r="C11" s="8">
         <v>1.03</v>
       </c>
-      <c r="I11" s="13" t="str">
+      <c r="I11" s="45" t="str">
         <f t="shared" si="2"/>
         <v>1F0A</v>
       </c>
-      <c r="J11" s="14">
+      <c r="J11" s="11">
         <f t="shared" si="3"/>
         <v>7946.24</v>
       </c>
-      <c r="K11" s="14">
+      <c r="K11" s="11">
         <v>0.97</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="20">
         <f t="shared" si="4"/>
         <v>1.1154999999999999</v>
       </c>
-      <c r="M11" s="9" t="str">
+      <c r="M11" s="24" t="str">
         <f t="shared" si="5"/>
         <v>23B2</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="27" t="str">
         <f t="shared" si="6"/>
+        <v>4764</v>
+      </c>
+      <c r="O11" s="30">
+        <f t="shared" si="7"/>
         <v>1.0669999999999999</v>
       </c>
-      <c r="O11" s="9" t="str">
-        <f t="shared" si="7"/>
+      <c r="P11" s="24" t="str">
+        <f t="shared" si="8"/>
         <v>2224</v>
       </c>
-      <c r="P11" s="9">
-        <f t="shared" si="8"/>
+      <c r="Q11" s="27" t="str">
+        <f t="shared" si="9"/>
+        <v>4449</v>
+      </c>
+      <c r="R11" s="30">
+        <f t="shared" si="10"/>
         <v>0.82450000000000001</v>
       </c>
-      <c r="Q11" s="9" t="str">
-        <f t="shared" si="9"/>
+      <c r="S11" s="24" t="str">
+        <f t="shared" si="11"/>
         <v>1A62</v>
       </c>
-      <c r="R11" s="9">
-        <f t="shared" si="10"/>
+      <c r="T11" s="27" t="str">
+        <f t="shared" si="12"/>
+        <v>34C4</v>
+      </c>
+      <c r="U11" s="30">
+        <f t="shared" si="13"/>
         <v>0.873</v>
       </c>
-      <c r="S11" s="9" t="str">
-        <f t="shared" si="11"/>
+      <c r="V11" s="24" t="str">
+        <f t="shared" si="14"/>
         <v>1BEF</v>
       </c>
-      <c r="T11" s="9">
-        <f t="shared" si="12"/>
+      <c r="W11" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>37DF</v>
+      </c>
+      <c r="X11" s="30">
+        <f t="shared" si="16"/>
         <v>1.0669999999999999</v>
       </c>
-      <c r="U11" s="9" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y11" s="33" t="str">
+        <f t="shared" si="17"/>
         <v>2224</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="str">
         <f t="shared" si="0"/>
         <v>2147</v>
@@ -1030,59 +1481,75 @@
       <c r="C12" s="8">
         <v>1.04</v>
       </c>
-      <c r="I12" s="13" t="str">
+      <c r="I12" s="45" t="str">
         <f t="shared" si="2"/>
         <v>1F5C</v>
       </c>
-      <c r="J12" s="14">
+      <c r="J12" s="11">
         <f t="shared" si="3"/>
         <v>8028.16</v>
       </c>
-      <c r="K12" s="14">
+      <c r="K12" s="11">
         <v>0.98</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="20">
         <f t="shared" si="4"/>
         <v>1.127</v>
       </c>
-      <c r="M12" s="9" t="str">
+      <c r="M12" s="24" t="str">
         <f t="shared" si="5"/>
         <v>2410</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="27" t="str">
         <f t="shared" si="6"/>
+        <v>4820</v>
+      </c>
+      <c r="O12" s="30">
+        <f t="shared" si="7"/>
         <v>1.0780000000000001</v>
       </c>
-      <c r="O12" s="9" t="str">
-        <f t="shared" si="7"/>
+      <c r="P12" s="24" t="str">
+        <f t="shared" si="8"/>
         <v>227E</v>
       </c>
-      <c r="P12" s="9">
-        <f t="shared" si="8"/>
+      <c r="Q12" s="27" t="str">
+        <f t="shared" si="9"/>
+        <v>44FD</v>
+      </c>
+      <c r="R12" s="30">
+        <f t="shared" si="10"/>
         <v>0.83299999999999996</v>
       </c>
-      <c r="Q12" s="9" t="str">
-        <f t="shared" si="9"/>
+      <c r="S12" s="24" t="str">
+        <f t="shared" si="11"/>
         <v>1AA7</v>
       </c>
-      <c r="R12" s="9">
-        <f t="shared" si="10"/>
+      <c r="T12" s="27" t="str">
+        <f t="shared" si="12"/>
+        <v>354F</v>
+      </c>
+      <c r="U12" s="30">
+        <f t="shared" si="13"/>
         <v>0.88200000000000001</v>
       </c>
-      <c r="S12" s="9" t="str">
-        <f t="shared" si="11"/>
+      <c r="V12" s="24" t="str">
+        <f t="shared" si="14"/>
         <v>1C39</v>
       </c>
-      <c r="T12" s="9">
-        <f t="shared" si="12"/>
+      <c r="W12" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>3872</v>
+      </c>
+      <c r="X12" s="30">
+        <f t="shared" si="16"/>
         <v>1.0780000000000001</v>
       </c>
-      <c r="U12" s="9" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y12" s="33" t="str">
+        <f t="shared" si="17"/>
         <v>227E</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="str">
         <f t="shared" si="0"/>
         <v>2199</v>
@@ -1094,59 +1561,75 @@
       <c r="C13" s="8">
         <v>1.05</v>
       </c>
-      <c r="I13" s="13" t="str">
+      <c r="I13" s="45" t="str">
         <f t="shared" si="2"/>
         <v>1FAE</v>
       </c>
-      <c r="J13" s="14">
+      <c r="J13" s="11">
         <f t="shared" si="3"/>
         <v>8110.08</v>
       </c>
-      <c r="K13" s="14">
+      <c r="K13" s="11">
         <v>0.99</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="20">
         <f t="shared" si="4"/>
         <v>1.1384999999999998</v>
       </c>
-      <c r="M13" s="9" t="str">
+      <c r="M13" s="24" t="str">
         <f t="shared" si="5"/>
         <v>246E</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="27" t="str">
         <f t="shared" si="6"/>
+        <v>48DD</v>
+      </c>
+      <c r="O13" s="30">
+        <f t="shared" si="7"/>
         <v>1.089</v>
       </c>
-      <c r="O13" s="9" t="str">
-        <f t="shared" si="7"/>
+      <c r="P13" s="24" t="str">
+        <f t="shared" si="8"/>
         <v>22D9</v>
       </c>
-      <c r="P13" s="9">
-        <f t="shared" si="8"/>
+      <c r="Q13" s="27" t="str">
+        <f t="shared" si="9"/>
+        <v>45B2</v>
+      </c>
+      <c r="R13" s="30">
+        <f t="shared" si="10"/>
         <v>0.84150000000000003</v>
       </c>
-      <c r="Q13" s="9" t="str">
-        <f t="shared" si="9"/>
+      <c r="S13" s="24" t="str">
+        <f t="shared" si="11"/>
         <v>1AED</v>
       </c>
-      <c r="R13" s="9">
-        <f t="shared" si="10"/>
+      <c r="T13" s="27" t="str">
+        <f t="shared" si="12"/>
+        <v>35DB</v>
+      </c>
+      <c r="U13" s="30">
+        <f t="shared" si="13"/>
         <v>0.89100000000000001</v>
       </c>
-      <c r="S13" s="9" t="str">
-        <f t="shared" si="11"/>
+      <c r="V13" s="24" t="str">
+        <f t="shared" si="14"/>
         <v>1C83</v>
       </c>
-      <c r="T13" s="9">
-        <f t="shared" si="12"/>
+      <c r="W13" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>3906</v>
+      </c>
+      <c r="X13" s="30">
+        <f t="shared" si="16"/>
         <v>1.089</v>
       </c>
-      <c r="U13" s="9" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y13" s="33" t="str">
+        <f t="shared" si="17"/>
         <v>22D9</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="str">
         <f t="shared" si="0"/>
         <v>21EB</v>
@@ -1158,405 +1641,517 @@
       <c r="C14" s="8">
         <v>1.06</v>
       </c>
-      <c r="I14" s="10" t="str">
+      <c r="I14" s="44" t="str">
         <f t="shared" si="2"/>
         <v>2000</v>
       </c>
-      <c r="J14" s="11">
+      <c r="J14" s="10">
         <f t="shared" si="3"/>
         <v>8192</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="10">
         <v>1</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="21">
         <f t="shared" si="4"/>
         <v>1.1499999999999999</v>
       </c>
-      <c r="M14" s="12" t="str">
+      <c r="M14" s="25" t="str">
         <f t="shared" si="5"/>
         <v>24CC</v>
       </c>
-      <c r="N14" s="12">
+      <c r="N14" s="26" t="str">
         <f t="shared" si="6"/>
+        <v>4999</v>
+      </c>
+      <c r="O14" s="31">
+        <f t="shared" si="7"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="O14" s="12" t="str">
-        <f t="shared" si="7"/>
+      <c r="P14" s="25" t="str">
+        <f t="shared" si="8"/>
         <v>2333</v>
       </c>
-      <c r="P14" s="12">
-        <f t="shared" si="8"/>
+      <c r="Q14" s="26" t="str">
+        <f t="shared" si="9"/>
+        <v>4666</v>
+      </c>
+      <c r="R14" s="31">
+        <f t="shared" si="10"/>
         <v>0.85</v>
       </c>
-      <c r="Q14" s="12" t="str">
-        <f t="shared" si="9"/>
+      <c r="S14" s="25" t="str">
+        <f t="shared" si="11"/>
         <v>1B33</v>
       </c>
-      <c r="R14" s="12">
-        <f t="shared" si="10"/>
+      <c r="T14" s="26" t="str">
+        <f t="shared" si="12"/>
+        <v>3666</v>
+      </c>
+      <c r="U14" s="31">
+        <f t="shared" si="13"/>
         <v>0.9</v>
       </c>
-      <c r="S14" s="12" t="str">
-        <f t="shared" si="11"/>
+      <c r="V14" s="25" t="str">
+        <f t="shared" si="14"/>
         <v>1CCC</v>
       </c>
-      <c r="T14" s="12">
-        <f t="shared" si="12"/>
+      <c r="W14" s="26" t="str">
+        <f t="shared" si="15"/>
+        <v>3999</v>
+      </c>
+      <c r="X14" s="31">
+        <f t="shared" si="16"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="U14" s="12" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y14" s="34" t="str">
+        <f t="shared" si="17"/>
         <v>2333</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="I15" s="13" t="str">
+    <row r="15" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="I15" s="45" t="str">
         <f t="shared" si="2"/>
         <v>2051</v>
       </c>
-      <c r="J15" s="14">
+      <c r="J15" s="11">
         <f t="shared" si="3"/>
         <v>8273.92</v>
       </c>
-      <c r="K15" s="14">
+      <c r="K15" s="11">
         <v>1.01</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="20">
         <f t="shared" si="4"/>
         <v>1.1615</v>
       </c>
-      <c r="M15" s="9" t="str">
+      <c r="M15" s="24" t="str">
         <f t="shared" si="5"/>
         <v>252B</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="27" t="str">
         <f t="shared" si="6"/>
+        <v>4A56</v>
+      </c>
+      <c r="O15" s="30">
+        <f t="shared" si="7"/>
         <v>1.1110000000000002</v>
       </c>
-      <c r="O15" s="9" t="str">
-        <f t="shared" si="7"/>
+      <c r="P15" s="24" t="str">
+        <f t="shared" si="8"/>
         <v>238D</v>
       </c>
-      <c r="P15" s="9">
-        <f t="shared" si="8"/>
+      <c r="Q15" s="27" t="str">
+        <f t="shared" si="9"/>
+        <v>471A</v>
+      </c>
+      <c r="R15" s="30">
+        <f t="shared" si="10"/>
         <v>0.85849999999999993</v>
       </c>
-      <c r="Q15" s="9" t="str">
-        <f t="shared" si="9"/>
+      <c r="S15" s="24" t="str">
+        <f t="shared" si="11"/>
         <v>1B78</v>
       </c>
-      <c r="R15" s="9">
-        <f t="shared" si="10"/>
+      <c r="T15" s="27" t="str">
+        <f t="shared" si="12"/>
+        <v>36F1</v>
+      </c>
+      <c r="U15" s="30">
+        <f t="shared" si="13"/>
         <v>0.90900000000000003</v>
       </c>
-      <c r="S15" s="9" t="str">
-        <f t="shared" si="11"/>
+      <c r="V15" s="24" t="str">
+        <f t="shared" si="14"/>
         <v>1D16</v>
       </c>
-      <c r="T15" s="9">
-        <f t="shared" si="12"/>
+      <c r="W15" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>3A2D</v>
+      </c>
+      <c r="X15" s="30">
+        <f t="shared" si="16"/>
         <v>1.1110000000000002</v>
       </c>
-      <c r="U15" s="9" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y15" s="33" t="str">
+        <f t="shared" si="17"/>
         <v>238D</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
+    <row r="16" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="17"/>
-      <c r="I16" s="13" t="str">
+      <c r="C16" s="14"/>
+      <c r="I16" s="45" t="str">
         <f t="shared" si="2"/>
         <v>20A3</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="11">
         <f t="shared" si="3"/>
         <v>8355.84</v>
       </c>
-      <c r="K16" s="14">
+      <c r="K16" s="11">
         <v>1.02</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="20">
         <f t="shared" si="4"/>
         <v>1.1729999999999998</v>
       </c>
-      <c r="M16" s="9" t="str">
+      <c r="M16" s="24" t="str">
         <f t="shared" si="5"/>
         <v>2589</v>
       </c>
-      <c r="N16" s="9">
+      <c r="N16" s="27" t="str">
         <f t="shared" si="6"/>
+        <v>4B12</v>
+      </c>
+      <c r="O16" s="30">
+        <f t="shared" si="7"/>
         <v>1.1220000000000001</v>
       </c>
-      <c r="O16" s="9" t="str">
-        <f t="shared" si="7"/>
+      <c r="P16" s="24" t="str">
+        <f t="shared" si="8"/>
         <v>23E7</v>
       </c>
-      <c r="P16" s="9">
-        <f t="shared" si="8"/>
+      <c r="Q16" s="27" t="str">
+        <f t="shared" si="9"/>
+        <v>47CE</v>
+      </c>
+      <c r="R16" s="30">
+        <f t="shared" si="10"/>
         <v>0.86699999999999999</v>
       </c>
-      <c r="Q16" s="9" t="str">
-        <f t="shared" si="9"/>
+      <c r="S16" s="24" t="str">
+        <f t="shared" si="11"/>
         <v>1BBE</v>
       </c>
-      <c r="R16" s="9">
-        <f t="shared" si="10"/>
+      <c r="T16" s="27" t="str">
+        <f t="shared" si="12"/>
+        <v>377C</v>
+      </c>
+      <c r="U16" s="30">
+        <f t="shared" si="13"/>
         <v>0.91800000000000004</v>
       </c>
-      <c r="S16" s="9" t="str">
-        <f t="shared" si="11"/>
+      <c r="V16" s="24" t="str">
+        <f t="shared" si="14"/>
         <v>1D60</v>
       </c>
-      <c r="T16" s="9">
-        <f t="shared" si="12"/>
+      <c r="W16" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>3AC0</v>
+      </c>
+      <c r="X16" s="30">
+        <f t="shared" si="16"/>
         <v>1.1220000000000001</v>
       </c>
-      <c r="U16" s="9" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y16" s="33" t="str">
+        <f t="shared" si="17"/>
         <v>23E7</v>
       </c>
     </row>
-    <row r="17" spans="1:21" ht="33" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:25" ht="33" x14ac:dyDescent="0.25">
+      <c r="A17" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="18"/>
-      <c r="I17" s="13" t="str">
+      <c r="C17" s="15"/>
+      <c r="I17" s="45" t="str">
         <f t="shared" si="2"/>
         <v>20F5</v>
       </c>
-      <c r="J17" s="14">
+      <c r="J17" s="11">
         <f t="shared" si="3"/>
         <v>8437.76</v>
       </c>
-      <c r="K17" s="14">
+      <c r="K17" s="11">
         <v>1.03</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="20">
         <f t="shared" si="4"/>
         <v>1.1844999999999999</v>
       </c>
-      <c r="M17" s="9" t="str">
+      <c r="M17" s="24" t="str">
         <f t="shared" si="5"/>
         <v>25E7</v>
       </c>
-      <c r="N17" s="9">
+      <c r="N17" s="27" t="str">
         <f t="shared" si="6"/>
+        <v>4BCE</v>
+      </c>
+      <c r="O17" s="30">
+        <f t="shared" si="7"/>
         <v>1.1330000000000002</v>
       </c>
-      <c r="O17" s="9" t="str">
-        <f t="shared" si="7"/>
+      <c r="P17" s="24" t="str">
+        <f t="shared" si="8"/>
         <v>2441</v>
       </c>
-      <c r="P17" s="9">
-        <f t="shared" si="8"/>
+      <c r="Q17" s="27" t="str">
+        <f t="shared" si="9"/>
+        <v>4883</v>
+      </c>
+      <c r="R17" s="30">
+        <f t="shared" si="10"/>
         <v>0.87549999999999994</v>
       </c>
-      <c r="Q17" s="9" t="str">
-        <f t="shared" si="9"/>
+      <c r="S17" s="24" t="str">
+        <f t="shared" si="11"/>
         <v>1C04</v>
       </c>
-      <c r="R17" s="9">
-        <f t="shared" si="10"/>
+      <c r="T17" s="27" t="str">
+        <f t="shared" si="12"/>
+        <v>3808</v>
+      </c>
+      <c r="U17" s="30">
+        <f t="shared" si="13"/>
         <v>0.92700000000000005</v>
       </c>
-      <c r="S17" s="9" t="str">
-        <f t="shared" si="11"/>
+      <c r="V17" s="24" t="str">
+        <f t="shared" si="14"/>
         <v>1DA9</v>
       </c>
-      <c r="T17" s="9">
-        <f t="shared" si="12"/>
+      <c r="W17" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>3B53</v>
+      </c>
+      <c r="X17" s="30">
+        <f t="shared" si="16"/>
         <v>1.1330000000000002</v>
       </c>
-      <c r="U17" s="9" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y17" s="33" t="str">
+        <f t="shared" si="17"/>
         <v>2441</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="19" t="s">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="I18" s="13" t="str">
+      <c r="C18" s="17"/>
+      <c r="I18" s="45" t="str">
         <f t="shared" si="2"/>
         <v>2147</v>
       </c>
-      <c r="J18" s="14">
+      <c r="J18" s="11">
         <f t="shared" si="3"/>
         <v>8519.68</v>
       </c>
-      <c r="K18" s="14">
+      <c r="K18" s="11">
         <v>1.04</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="20">
         <f t="shared" si="4"/>
         <v>1.196</v>
       </c>
-      <c r="M18" s="9" t="str">
+      <c r="M18" s="24" t="str">
         <f t="shared" si="5"/>
         <v>2645</v>
       </c>
-      <c r="N18" s="9">
+      <c r="N18" s="27" t="str">
         <f t="shared" si="6"/>
+        <v>4C8B</v>
+      </c>
+      <c r="O18" s="30">
+        <f t="shared" si="7"/>
         <v>1.1440000000000001</v>
       </c>
-      <c r="O18" s="9" t="str">
-        <f t="shared" si="7"/>
+      <c r="P18" s="24" t="str">
+        <f t="shared" si="8"/>
         <v>249B</v>
       </c>
-      <c r="P18" s="9">
-        <f t="shared" si="8"/>
+      <c r="Q18" s="27" t="str">
+        <f t="shared" si="9"/>
+        <v>4937</v>
+      </c>
+      <c r="R18" s="30">
+        <f t="shared" si="10"/>
         <v>0.88400000000000001</v>
       </c>
-      <c r="Q18" s="9" t="str">
-        <f t="shared" si="9"/>
+      <c r="S18" s="24" t="str">
+        <f t="shared" si="11"/>
         <v>1C49</v>
       </c>
-      <c r="R18" s="9">
-        <f t="shared" si="10"/>
+      <c r="T18" s="27" t="str">
+        <f t="shared" si="12"/>
+        <v>3893</v>
+      </c>
+      <c r="U18" s="30">
+        <f t="shared" si="13"/>
         <v>0.93600000000000005</v>
       </c>
-      <c r="S18" s="9" t="str">
-        <f t="shared" si="11"/>
+      <c r="V18" s="24" t="str">
+        <f t="shared" si="14"/>
         <v>1DF3</v>
       </c>
-      <c r="T18" s="9">
-        <f t="shared" si="12"/>
+      <c r="W18" s="27" t="str">
+        <f t="shared" si="15"/>
+        <v>3BE7</v>
+      </c>
+      <c r="X18" s="30">
+        <f t="shared" si="16"/>
         <v>1.1440000000000001</v>
       </c>
-      <c r="U18" s="9" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y18" s="33" t="str">
+        <f t="shared" si="17"/>
         <v>249B</v>
       </c>
     </row>
-    <row r="19" spans="1:21" ht="33" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="19" t="s">
+    <row r="19" spans="1:25" ht="33" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
+      <c r="B19" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="I19" s="10" t="str">
+      <c r="C19" s="17"/>
+      <c r="I19" s="44" t="str">
         <f t="shared" si="2"/>
         <v>2199</v>
       </c>
-      <c r="J19" s="11">
+      <c r="J19" s="10">
         <f t="shared" si="3"/>
         <v>8601.6</v>
       </c>
-      <c r="K19" s="11">
+      <c r="K19" s="10">
         <v>1.05</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="21">
         <f t="shared" si="4"/>
         <v>1.2075</v>
       </c>
-      <c r="M19" s="12" t="str">
+      <c r="M19" s="25" t="str">
         <f t="shared" si="5"/>
         <v>26A3</v>
       </c>
-      <c r="N19" s="12">
+      <c r="N19" s="26" t="str">
         <f t="shared" si="6"/>
+        <v>4D47</v>
+      </c>
+      <c r="O19" s="31">
+        <f t="shared" si="7"/>
         <v>1.1550000000000002</v>
       </c>
-      <c r="O19" s="12" t="str">
-        <f t="shared" si="7"/>
+      <c r="P19" s="25" t="str">
+        <f t="shared" si="8"/>
         <v>24F5</v>
       </c>
-      <c r="P19" s="12">
-        <f t="shared" si="8"/>
+      <c r="Q19" s="26" t="str">
+        <f t="shared" si="9"/>
+        <v>49EB</v>
+      </c>
+      <c r="R19" s="31">
+        <f t="shared" si="10"/>
         <v>0.89249999999999996</v>
       </c>
-      <c r="Q19" s="12" t="str">
-        <f t="shared" si="9"/>
+      <c r="S19" s="25" t="str">
+        <f t="shared" si="11"/>
         <v>1C8F</v>
       </c>
-      <c r="R19" s="12">
-        <f t="shared" si="10"/>
+      <c r="T19" s="26" t="str">
+        <f t="shared" si="12"/>
+        <v>391E</v>
+      </c>
+      <c r="U19" s="31">
+        <f t="shared" si="13"/>
         <v>0.94500000000000006</v>
       </c>
-      <c r="S19" s="12" t="str">
-        <f t="shared" si="11"/>
+      <c r="V19" s="25" t="str">
+        <f t="shared" si="14"/>
         <v>1E3D</v>
       </c>
-      <c r="T19" s="12">
-        <f t="shared" si="12"/>
+      <c r="W19" s="26" t="str">
+        <f t="shared" si="15"/>
+        <v>3C7A</v>
+      </c>
+      <c r="X19" s="31">
+        <f t="shared" si="16"/>
         <v>1.1550000000000002</v>
       </c>
-      <c r="U19" s="12" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y19" s="34" t="str">
+        <f t="shared" si="17"/>
         <v>24F5</v>
       </c>
     </row>
-    <row r="20" spans="1:21" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22" t="s">
+    <row r="20" spans="1:25" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="18"/>
+      <c r="B20" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="I20" s="13" t="str">
+      <c r="C20" s="18"/>
+      <c r="I20" s="46" t="str">
         <f t="shared" si="2"/>
         <v>21EB</v>
       </c>
-      <c r="J20" s="14">
+      <c r="J20" s="47">
         <f t="shared" si="3"/>
         <v>8683.52</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="47">
         <v>1.06</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="48">
         <f t="shared" si="4"/>
         <v>1.2189999999999999</v>
       </c>
-      <c r="M20" s="9" t="str">
+      <c r="M20" s="28" t="str">
         <f t="shared" si="5"/>
         <v>2702</v>
       </c>
-      <c r="N20" s="9">
+      <c r="N20" s="29" t="str">
         <f t="shared" si="6"/>
+        <v>4E04</v>
+      </c>
+      <c r="O20" s="49">
+        <f t="shared" si="7"/>
         <v>1.1660000000000001</v>
       </c>
-      <c r="O20" s="9" t="str">
-        <f t="shared" si="7"/>
+      <c r="P20" s="28" t="str">
+        <f t="shared" si="8"/>
         <v>254F</v>
       </c>
-      <c r="P20" s="9">
-        <f t="shared" si="8"/>
+      <c r="Q20" s="29" t="str">
+        <f t="shared" si="9"/>
+        <v>4A9F</v>
+      </c>
+      <c r="R20" s="49">
+        <f t="shared" si="10"/>
         <v>0.90100000000000002</v>
       </c>
-      <c r="Q20" s="9" t="str">
-        <f t="shared" si="9"/>
+      <c r="S20" s="28" t="str">
+        <f t="shared" si="11"/>
         <v>1CD4</v>
       </c>
-      <c r="R20" s="9">
-        <f t="shared" si="10"/>
+      <c r="T20" s="29" t="str">
+        <f t="shared" si="12"/>
+        <v>39A9</v>
+      </c>
+      <c r="U20" s="49">
+        <f t="shared" si="13"/>
         <v>0.95400000000000007</v>
       </c>
-      <c r="S20" s="9" t="str">
-        <f t="shared" si="11"/>
+      <c r="V20" s="28" t="str">
+        <f t="shared" si="14"/>
         <v>1E87</v>
       </c>
-      <c r="T20" s="9">
-        <f t="shared" si="12"/>
+      <c r="W20" s="29" t="str">
+        <f t="shared" si="15"/>
+        <v>3D0E</v>
+      </c>
+      <c r="X20" s="49">
+        <f t="shared" si="16"/>
         <v>1.1660000000000001</v>
       </c>
-      <c r="U20" s="9" t="str">
-        <f t="shared" si="13"/>
+      <c r="Y20" s="35" t="str">
+        <f t="shared" si="17"/>
         <v>254F</v>
       </c>
     </row>

</xml_diff>